<commit_message>
Fixed issue with audio waveform clipping. Improved documentation, and made the lookup table more efficient by eliminating redundant information.
</commit_message>
<xml_diff>
--- a/Timer Value Comparisons for Baud and Tone Generation.xlsx
+++ b/Timer Value Comparisons for Baud and Tone Generation.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15da9958d5653d7c/Git/ptSolar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="8_{EFBF5CDD-90CD-49C6-81E3-4432BDE0BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36890C22-4F48-4F19-9EB5-26255A381068}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="8_{EFBF5CDD-90CD-49C6-81E3-4432BDE0BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1584BD8F-56D5-48B5-AC7F-8C2759F0B805}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{DF6E09ED-C946-4170-A532-3478E12C41B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{DF6E09ED-C946-4170-A532-3478E12C41B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Timer1 Calcs" sheetId="1" r:id="rId1"/>
-    <sheet name="Sin Table" sheetId="2" r:id="rId2"/>
+    <sheet name="Truncated Sine Table" sheetId="3" r:id="rId1"/>
+    <sheet name="Timer1 Calcs" sheetId="1" r:id="rId2"/>
+    <sheet name="Sine Table" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>BG</t>
   </si>
@@ -89,13 +90,19 @@
   <si>
     <t>arySin[] = {</t>
   </si>
+  <si>
+    <t>Max Value</t>
+  </si>
+  <si>
+    <t>(set to 255 or less). This need to be at or less than the value in OCR2A or else you'll have overflow issues in the PWM generation.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="164" formatCode="0.000%"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -128,7 +135,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,6 +151,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -462,6 +473,1442 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7676FD-96D6-4691-856B-BD53CD89FC77}">
+  <dimension ref="A1:K65"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:K17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="10" max="10" width="12.21875" customWidth="1"/>
+    <col min="11" max="11" width="46.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <f>(A2/256) * 360</f>
+        <v>1.40625</v>
+      </c>
+      <c r="C2">
+        <f>B2*PI()/180</f>
+        <v>2.4543692606170259E-2</v>
+      </c>
+      <c r="D2">
+        <f>SIN(C2)</f>
+        <v>2.4541228522912288E-2</v>
+      </c>
+      <c r="E2">
+        <f>ROUND(($J$4*(D2)), 0)</f>
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2">
+        <v>200</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <f t="shared" ref="B3:B65" si="0">(A3/256) * 360</f>
+        <v>2.8125</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C65" si="1">B3*PI()/180</f>
+        <v>4.9087385212340517E-2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D65" si="2">SIN(C3)</f>
+        <v>4.9067674327418015E-2</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E65" si="3">ROUND(($J$4*(D3)), 0)</f>
+        <v>5</v>
+      </c>
+      <c r="I3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <f>ROUND((255 - J2) / 2, 0)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f t="shared" si="0"/>
+        <v>4.21875</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="1"/>
+        <v>7.3631077818510776E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>7.3564563599667426E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4">
+        <f>INT(J2/2)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>5.625</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="1"/>
+        <v>9.8174770424681035E-2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="2"/>
+        <v>9.8017140329560604E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>7.03125</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="1"/>
+        <v>0.12271846303085129</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>0.1224106751992162</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>8.4375</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="1"/>
+        <v>0.14726215563702155</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="2"/>
+        <v>0.14673047445536175</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>9.84375</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="1"/>
+        <v>0.17180584824319181</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="2"/>
+        <v>0.17096188876030122</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="K8" t="str">
+        <f>_xlfn.CONCAT("uint8_t arySin[] = {", E2, ", ", E3, ", ", E4, ", ", E5, ", ", E6, ", ", E7, ", ", E8, ", ", E9, ", ", E10, ", ", E11, ", ")</f>
+        <v xml:space="preserve">uint8_t arySin[] = {2, 5, 7, 10, 12, 15, 17, 20, 22, 24, </v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>11.25</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="1"/>
+        <v>0.19634954084936207</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="2"/>
+        <v>0.19509032201612825</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="K9" t="str">
+        <f>_xlfn.CONCAT(E12, ", ", E13, ", ", E14, ", ", E15, ", ", E16, ", ", E17, ", ", E18, ", ", E19, ", ", E20, ", ", E21, ", ")</f>
+        <v xml:space="preserve">27, 29, 31, 34, 36, 38, 41, 43, 45, 47, </v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>12.65625</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="1"/>
+        <v>0.2208932334555323</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="2"/>
+        <v>0.21910124015686977</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="K10" t="str">
+        <f>_xlfn.CONCAT(E22, ", ", E23, ", ", E24, ", ", E25, ", ", E26, ", ", E27, ", ", E28, ", ", E29, ", ", E30, ", ", E31, ", ")</f>
+        <v xml:space="preserve">49, 51, 53, 56, 58, 60, 62, 63, 65, 67, </v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>14.0625</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="1"/>
+        <v>0.24543692606170259</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="2"/>
+        <v>0.24298017990326387</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="K11" t="str">
+        <f>_xlfn.CONCAT(E32, ", ", E33, ", ", E34, ", ", E35, ", ", E36, ", ", E37, ", ", E38, ", ", E39, ", ", E40, ", ", E41, ", ")</f>
+        <v xml:space="preserve">69, 71, 72, 74, 76, 77, 79, 80, 82, 83, </v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>15.46875</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>0.26998061866787287</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="2"/>
+        <v>0.26671275747489842</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="K12" t="str">
+        <f>_xlfn.CONCAT(E42, ", ", E43, ", ", E44, ", ", E45, ", ", E46, ", ", E47, ", ", E48, ", ", E49, ", ", E50, ", ", E51, ", ")</f>
+        <v xml:space="preserve">84, 86, 87, 88, 89, 90, 91, 92, 93, 94, </v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>16.875</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>0.2945243112740431</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>0.29028467725446233</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="K13" t="str">
+        <f>_xlfn.CONCAT(E52, ", ", E53, ", ", E54, ", ", E55, ", ", E56, ", ", E57, ", ", E58, ", ", E59, ", ", E60, ", ", E61, ", ")</f>
+        <v xml:space="preserve">95, 96, 96, 97, 98, 98, 99, 99, 99, 100, </v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>18.28125</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>0.31906800388021339</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>0.31368174039889152</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="K14" t="str">
+        <f>_xlfn.CONCAT(E62, ", ", E63, ", ", E64, ", ", E65, "};" )</f>
+        <v>100, 100, 100, 100};</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>19.6875</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>0.34361169648638362</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="2"/>
+        <v>0.33688985339222005</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>21.09375</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.36815538909255391</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="2"/>
+        <v>0.35989503653498817</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>22.5</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>0.39269908169872414</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="2"/>
+        <v>0.38268343236508978</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="K17" t="str">
+        <f>_xlfn.CONCAT("uint8_t ref = ", INT(J2/2), ";")</f>
+        <v>uint8_t ref = 100;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>23.90625</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>0.41724277430489437</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="2"/>
+        <v>0.40524131400498981</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>25.3125</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>0.4417864669110646</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="2"/>
+        <v>0.42755509343028203</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>26.71875</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>0.46633015951723494</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="2"/>
+        <v>0.4496113296546066</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>28.125</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>0.49087385212340517</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>0.47139673682599764</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>29.53125</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="1"/>
+        <v>0.51541754472957535</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="2"/>
+        <v>0.49289819222978393</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>30.9375</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="1"/>
+        <v>0.53996123733574575</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="2"/>
+        <v>0.51410274419322177</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="3"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>32.34375</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="1"/>
+        <v>0.56450492994191592</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="2"/>
+        <v>0.53499761988709715</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>33.75</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="1"/>
+        <v>0.58904862254808621</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="2"/>
+        <v>0.55557023301960218</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>35.15625</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="1"/>
+        <v>0.6135923151542565</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="2"/>
+        <v>0.57580819141784534</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="3"/>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>36.5625</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="1"/>
+        <v>0.63813600776042678</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="2"/>
+        <v>0.59569930449243336</v>
+      </c>
+      <c r="E27">
+        <f t="shared" si="3"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>37.96875</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="1"/>
+        <v>0.66267970036659696</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="2"/>
+        <v>0.61523159058062682</v>
+      </c>
+      <c r="E28">
+        <f t="shared" si="3"/>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>39.375</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="1"/>
+        <v>0.68722339297276724</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="2"/>
+        <v>0.63439328416364549</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="3"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>40.78125</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="1"/>
+        <v>0.71176708557893753</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="2"/>
+        <v>0.65317284295377676</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>42.1875</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="1"/>
+        <v>0.73631077818510782</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="2"/>
+        <v>0.67155895484701844</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="3"/>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>43.59375</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="1"/>
+        <v>0.76085447079127799</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="2"/>
+        <v>0.68954054473706683</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C33">
+        <f t="shared" si="1"/>
+        <v>0.78539816339744828</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="2"/>
+        <v>0.70710678118654746</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>46.40625</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="1"/>
+        <v>0.80994185600361857</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="2"/>
+        <v>0.72424708295146689</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>47.8125</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="1"/>
+        <v>0.83448554860978874</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="2"/>
+        <v>0.74095112535495899</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>49.21875</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="1"/>
+        <v>0.85902924121595903</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="2"/>
+        <v>0.75720884650648446</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>50.625</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="1"/>
+        <v>0.8835729338221292</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="2"/>
+        <v>0.77301045336273688</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="3"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>52.03125</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="1"/>
+        <v>0.9081166264282996</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>0.78834642762660623</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>53.4375</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="1"/>
+        <v>0.93266031903446989</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>0.80320753148064494</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>54.84375</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="1"/>
+        <v>0.95720401164064006</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>0.81758481315158371</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>56.25</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="1"/>
+        <v>0.98174770424681035</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>0.83146961230254524</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="3"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>57.65625</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="1"/>
+        <v>1.0062913968529807</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>0.84485356524970712</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="3"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>59.0625</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="1"/>
+        <v>1.0308350894591507</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>0.85772861000027201</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="3"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>60.46875</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="1"/>
+        <v>1.0553787820653211</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>0.87008699110871135</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="3"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>61.875</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="1"/>
+        <v>1.0799224746714915</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>0.88192126434835505</v>
+      </c>
+      <c r="E45">
+        <f t="shared" si="3"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>63.28125</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="1"/>
+        <v>1.1044661672776617</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>0.89322430119551532</v>
+      </c>
+      <c r="E46">
+        <f t="shared" si="3"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>64.6875</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="1"/>
+        <v>1.1290098598838318</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>0.90398929312344334</v>
+      </c>
+      <c r="E47">
+        <f t="shared" si="3"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>66.09375</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="1"/>
+        <v>1.1535535524900022</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>0.91420975570353069</v>
+      </c>
+      <c r="E48">
+        <f t="shared" si="3"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>67.5</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="1"/>
+        <v>1.1780972450961724</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>0.92387953251128674</v>
+      </c>
+      <c r="E49">
+        <f t="shared" si="3"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>68.90625</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="1"/>
+        <v>1.2026409377023426</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>0.93299279883473885</v>
+      </c>
+      <c r="E50">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>70.3125</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="1"/>
+        <v>1.227184630308513</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>0.94154406518302081</v>
+      </c>
+      <c r="E51">
+        <f t="shared" si="3"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>71.71875</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="1"/>
+        <v>1.2517283229146832</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>0.94952818059303667</v>
+      </c>
+      <c r="E52">
+        <f t="shared" si="3"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>73.125</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="1"/>
+        <v>1.2762720155208536</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>0.95694033573220894</v>
+      </c>
+      <c r="E53">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>74.53125</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="1"/>
+        <v>1.3008157081270237</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>0.96377606579543984</v>
+      </c>
+      <c r="E54">
+        <f t="shared" si="3"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>75.9375</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="1"/>
+        <v>1.3253594007331939</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>0.97003125319454397</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>77.34375</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="1"/>
+        <v>1.3499030933393643</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>0.97570213003852857</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <f t="shared" si="0"/>
+        <v>78.75</v>
+      </c>
+      <c r="C57">
+        <f t="shared" si="1"/>
+        <v>1.3744467859455345</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>0.98078528040323043</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="3"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <f t="shared" si="0"/>
+        <v>80.15625</v>
+      </c>
+      <c r="C58">
+        <f t="shared" si="1"/>
+        <v>1.3989904785517047</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>0.98527764238894122</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <f t="shared" si="0"/>
+        <v>81.5625</v>
+      </c>
+      <c r="C59">
+        <f t="shared" si="1"/>
+        <v>1.4235341711578751</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>0.98917650996478101</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <f t="shared" si="0"/>
+        <v>82.96875</v>
+      </c>
+      <c r="C60">
+        <f t="shared" si="1"/>
+        <v>1.4480778637640452</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>0.99247953459870997</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="3"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <f t="shared" si="0"/>
+        <v>84.375</v>
+      </c>
+      <c r="C61">
+        <f t="shared" si="1"/>
+        <v>1.4726215563702156</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>0.99518472667219693</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <f t="shared" si="0"/>
+        <v>85.78125</v>
+      </c>
+      <c r="C62">
+        <f t="shared" si="1"/>
+        <v>1.4971652489763856</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>0.99729045667869021</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63">
+        <f t="shared" si="0"/>
+        <v>87.1875</v>
+      </c>
+      <c r="C63">
+        <f t="shared" si="1"/>
+        <v>1.521708941582556</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>0.99879545620517241</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64">
+        <f t="shared" si="0"/>
+        <v>88.59375</v>
+      </c>
+      <c r="C64">
+        <f t="shared" si="1"/>
+        <v>1.5462526341887264</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>0.99969881869620425</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <f t="shared" si="0"/>
+        <v>90</v>
+      </c>
+      <c r="C65">
+        <f t="shared" si="1"/>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4B8AD3-CD47-4B54-BDA7-EF9D63D27F55}">
   <dimension ref="A1:G18"/>
   <sheetViews>
@@ -1011,12 +2458,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF094F3-9C97-46C0-BFFA-1F369A2C5E35}">
   <dimension ref="A1:K257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:K33"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:XFD257"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed a typo, and unded the compressed audio waveform. It was causing the audio tones to drop in frequency. Likely just needs PROGMEM set on the array.
</commit_message>
<xml_diff>
--- a/Timer Value Comparisons for Baud and Tone Generation.xlsx
+++ b/Timer Value Comparisons for Baud and Tone Generation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15da9958d5653d7c/Git/ptSolar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="8_{EFBF5CDD-90CD-49C6-81E3-4432BDE0BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1584BD8F-56D5-48B5-AC7F-8C2759F0B805}"/>
+  <xr:revisionPtr revIDLastSave="128" documentId="8_{EFBF5CDD-90CD-49C6-81E3-4432BDE0BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC5A0A6D-31BA-4C44-9E69-F669FB3B472D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{DF6E09ED-C946-4170-A532-3478E12C41B6}"/>
+    <workbookView xWindow="-24684" yWindow="-108" windowWidth="24792" windowHeight="13320" activeTab="2" xr2:uid="{DF6E09ED-C946-4170-A532-3478E12C41B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Truncated Sine Table" sheetId="3" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>BG</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>(set to 255 or less)</t>
-  </si>
-  <si>
-    <t>arySin[] = {</t>
   </si>
   <si>
     <t>Max Value</t>
@@ -476,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7676FD-96D6-4691-856B-BD53CD89FC77}">
   <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8:K17"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,13 +521,13 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J2">
         <v>200</v>
       </c>
       <c r="K2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
@@ -2462,8 +2459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF094F3-9C97-46C0-BFFA-1F369A2C5E35}">
   <dimension ref="A1:K257"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:XFD257"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8:K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2506,14 +2503,14 @@
         <v>2.4541228522912288E-2</v>
       </c>
       <c r="E2">
-        <f>ROUND(($J$4*(D2+1))+$J$3, 0)</f>
-        <v>131</v>
+        <f>ROUND(($J$4*(D2))+$J$3, 0)</f>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
         <v>11</v>
       </c>
       <c r="J2">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="K2" t="s">
         <v>15</v>
@@ -2536,15 +2533,15 @@
         <v>4.9067674327418015E-2</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E66" si="3">ROUND(($J$4*(D3+1))+$J$3, 0)</f>
-        <v>134</v>
+        <f t="shared" ref="E3:E66" si="3">ROUND(($J$4*(D3))+$J$3, 0)</f>
+        <v>105</v>
       </c>
       <c r="I3" t="s">
         <v>12</v>
       </c>
       <c r="J3">
-        <f>ROUND((255 - J2) / 2, 0)</f>
-        <v>5</v>
+        <f>ROUND(J2/2,0)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
@@ -2565,14 +2562,14 @@
       </c>
       <c r="E4">
         <f t="shared" si="3"/>
-        <v>137</v>
+        <v>107</v>
       </c>
       <c r="I4" t="s">
         <v>14</v>
       </c>
       <c r="J4">
-        <f>ROUND(J2/2, 0)</f>
-        <v>123</v>
+        <f>INT(J2/2)</f>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
@@ -2593,7 +2590,7 @@
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
@@ -2614,7 +2611,7 @@
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>143</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -2635,7 +2632,7 @@
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>146</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
@@ -2656,14 +2653,11 @@
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>149</v>
-      </c>
-      <c r="J8" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="K8" t="str">
-        <f>_xlfn.CONCAT(E2, ", ", E3, ", ", E4, ", ", E5, ", ", E6, ", ", E7, ", ", E8, ", ", E9, ", ", E10, ", ", E11, ", ")</f>
-        <v xml:space="preserve">131, 134, 137, 140, 143, 146, 149, 152, 155, 158, </v>
+        <f>_xlfn.CONCAT("uint8_t arySin[] = {", E2, ", ", E3, ", ", E4, ", ", E5, ", ", E6, ", ", E7, ", ", E8, ", ", E9, ", ", E10, ", ", E11, ", ")</f>
+        <v xml:space="preserve">uint8_t arySin[] = {102, 105, 107, 110, 112, 115, 117, 120, 122, 124, </v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
@@ -2684,11 +2678,11 @@
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="K9" t="str">
         <f>_xlfn.CONCAT(E12, ", ", E13, ", ", E14, ", ", E15, ", ", E16, ", ", E17, ", ", E18, ", ", E19, ", ", E20, ", ", E21, ", ")</f>
-        <v xml:space="preserve">161, 164, 167, 169, 172, 175, 178, 181, 183, 186, </v>
+        <v xml:space="preserve">127, 129, 131, 134, 136, 138, 141, 143, 145, 147, </v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
@@ -2709,11 +2703,11 @@
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
-        <v>155</v>
+        <v>122</v>
       </c>
       <c r="K10" t="str">
         <f>_xlfn.CONCAT(E22, ", ", E23, ", ", E24, ", ", E25, ", ", E26, ", ", E27, ", ", E28, ", ", E29, ", ", E30, ", ", E31, ", ")</f>
-        <v xml:space="preserve">189, 191, 194, 196, 199, 201, 204, 206, 208, 211, </v>
+        <v xml:space="preserve">149, 151, 153, 156, 158, 160, 162, 163, 165, 167, </v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
@@ -2734,11 +2728,11 @@
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
-        <v>158</v>
+        <v>124</v>
       </c>
       <c r="K11" t="str">
         <f>_xlfn.CONCAT(E32, ", ", E33, ", ", E34, ", ", E35, ", ", E36, ", ", E37, ", ", E38, ", ", E39, ", ", E40, ", ", E41, ", ")</f>
-        <v xml:space="preserve">213, 215, 217, 219, 221, 223, 225, 227, 229, 230, </v>
+        <v xml:space="preserve">169, 171, 172, 174, 176, 177, 179, 180, 182, 183, </v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
@@ -2759,11 +2753,11 @@
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>161</v>
+        <v>127</v>
       </c>
       <c r="K12" t="str">
         <f>_xlfn.CONCAT(E42, ", ", E43, ", ", E44, ", ", E45, ", ", E46, ", ", E47, ", ", E48, ", ", E49, ", ", E50, ", ", E51, ", ")</f>
-        <v xml:space="preserve">232, 234, 235, 236, 238, 239, 240, 242, 243, 244, </v>
+        <v xml:space="preserve">184, 186, 187, 188, 189, 190, 191, 192, 193, 194, </v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -2784,11 +2778,11 @@
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="K13" t="str">
         <f>_xlfn.CONCAT(E52, ", ", E53, ", ", E54, ", ", E55, ", ", E56, ", ", E57, ", ", E58, ", ", E59, ", ", E60, ", ", E61, ", ")</f>
-        <v xml:space="preserve">245, 246, 247, 247, 248, 249, 249, 250, 250, 250, </v>
+        <v xml:space="preserve">195, 196, 196, 197, 198, 198, 199, 199, 199, 200, </v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -2809,11 +2803,11 @@
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>167</v>
+        <v>131</v>
       </c>
       <c r="K14" t="str">
         <f>_xlfn.CONCAT(E62, ", ", E63, ", ", E64, ", ", E65, ", ", E66, ", ", E67, ", ", E68, ", ", E69, ", ", E70, ", ", E71, ", ")</f>
-        <v xml:space="preserve">251, 251, 251, 251, 251, 251, 251, 250, 250, 250, </v>
+        <v xml:space="preserve">200, 200, 200, 200, 200, 200, 200, 200, 199, 199, </v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
@@ -2834,11 +2828,11 @@
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="K15" t="str">
         <f>_xlfn.CONCAT(E72, ", ", E73, ", ", E74, ", ", E75, ", ", E76, ", ", E77, ", ", E78, ", ", E79, ", ", E80, ", ", E81, ", ")</f>
-        <v xml:space="preserve">249, 249, 248, 247, 247, 246, 245, 244, 243, 242, </v>
+        <v xml:space="preserve">199, 198, 198, 197, 196, 196, 195, 194, 193, 192, </v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
@@ -2859,11 +2853,11 @@
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
-        <v>172</v>
+        <v>136</v>
       </c>
       <c r="K16" t="str">
         <f>_xlfn.CONCAT(E82, ", ", E83, ", ", E84, ", ", E85, ", ", E86, ", ", E87, ", ", E88, ", ", E89, ", ", E90, ", ", E91, ", ")</f>
-        <v xml:space="preserve">240, 239, 238, 236, 235, 234, 232, 230, 229, 227, </v>
+        <v xml:space="preserve">191, 190, 189, 188, 187, 186, 184, 183, 182, 180, </v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
@@ -2884,11 +2878,11 @@
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="K17" t="str">
         <f>_xlfn.CONCAT(E92, ", ", E93, ", ", E94, ", ", E95, ", ", E96, ", ", E97, ", ", E98, ", ", E99, ", ", E100, ", ", E101, ", ")</f>
-        <v xml:space="preserve">225, 223, 221, 219, 217, 215, 213, 211, 208, 206, </v>
+        <v xml:space="preserve">179, 177, 176, 174, 172, 171, 169, 167, 165, 163, </v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
@@ -2909,11 +2903,11 @@
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
-        <v>178</v>
+        <v>141</v>
       </c>
       <c r="K18" t="str">
         <f>_xlfn.CONCAT(E102, ", ", E103, ", ", E104, ", ", E105, ", ", E106, ", ", E107, ", ", E108, ", ", E109, ", ", E110, ", ", E111, ", ")</f>
-        <v xml:space="preserve">204, 201, 199, 196, 194, 191, 189, 186, 183, 181, </v>
+        <v xml:space="preserve">162, 160, 158, 156, 153, 151, 149, 147, 145, 143, </v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
@@ -2934,11 +2928,11 @@
       </c>
       <c r="E19">
         <f t="shared" si="3"/>
-        <v>181</v>
+        <v>143</v>
       </c>
       <c r="K19" t="str">
         <f>_xlfn.CONCAT(E112, ", ", E113, ", ", E114, ", ", E115, ", ", E116, ", ", E117, ", ", E118, ", ", E119, ", ", E120, ", ", E121, ", ")</f>
-        <v xml:space="preserve">178, 175, 172, 169, 167, 164, 161, 158, 155, 152, </v>
+        <v xml:space="preserve">141, 138, 136, 134, 131, 129, 127, 124, 122, 120, </v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
@@ -2959,11 +2953,11 @@
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
-        <v>183</v>
+        <v>145</v>
       </c>
       <c r="K20" t="str">
         <f>_xlfn.CONCAT(E122, ", ", E123, ", ", E124, ", ", E125, ", ", E126, ", ", E127, ", ", E128, ", ", E129, ", ", E130, ", ", E131, ", ")</f>
-        <v xml:space="preserve">149, 146, 143, 140, 137, 134, 131, 128, 125, 122, </v>
+        <v xml:space="preserve">117, 115, 112, 110, 107, 105, 102, 100, 98, 95, </v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
@@ -2984,11 +2978,11 @@
       </c>
       <c r="E21">
         <f t="shared" si="3"/>
-        <v>186</v>
+        <v>147</v>
       </c>
       <c r="K21" t="str">
         <f>_xlfn.CONCAT(E132, ", ", E133, ", ", E134, ", ", E135, ", ", E136, ", ", E137, ", ", E138, ", ", E139, ", ", E140, ", ", E141, ", ")</f>
-        <v xml:space="preserve">119, 116, 113, 110, 107, 104, 101, 98, 95, 92, </v>
+        <v xml:space="preserve">93, 90, 88, 85, 83, 80, 78, 76, 73, 71, </v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -3009,11 +3003,11 @@
       </c>
       <c r="E22">
         <f t="shared" si="3"/>
-        <v>189</v>
+        <v>149</v>
       </c>
       <c r="K22" t="str">
         <f>_xlfn.CONCAT(E142, ", ", E143, ", ", E144, ", ", E145, ", ", E146, ", ", E147, ", ", E148, ", ", E149, ", ", E150, ", ", E151, ", ")</f>
-        <v xml:space="preserve">89, 87, 84, 81, 78, 75, 73, 70, 67, 65, </v>
+        <v xml:space="preserve">69, 66, 64, 62, 59, 57, 55, 53, 51, 49, </v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
@@ -3034,11 +3028,11 @@
       </c>
       <c r="E23">
         <f t="shared" si="3"/>
-        <v>191</v>
+        <v>151</v>
       </c>
       <c r="K23" t="str">
         <f>_xlfn.CONCAT(E152, ", ", E153, ", ", E154, ", ", E155, ", ", E156, ", ", E157, ", ", E158, ", ", E159, ", ", E160, ", ", E161, ", ")</f>
-        <v xml:space="preserve">62, 60, 57, 55, 52, 50, 48, 45, 43, 41, </v>
+        <v xml:space="preserve">47, 44, 42, 40, 38, 37, 35, 33, 31, 29, </v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
@@ -3059,11 +3053,11 @@
       </c>
       <c r="E24">
         <f t="shared" si="3"/>
-        <v>194</v>
+        <v>153</v>
       </c>
       <c r="K24" t="str">
         <f>_xlfn.CONCAT(E162, ", ", E163, ", ", E164, ", ", E165, ", ", E166, ", ", E167, ", ", E168, ", ", E169, ", ", E170, ", ", E171, ", ")</f>
-        <v xml:space="preserve">39, 37, 35, 33, 31, 29, 27, 26, 24, 22, </v>
+        <v xml:space="preserve">28, 26, 24, 23, 21, 20, 18, 17, 16, 14, </v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
@@ -3084,11 +3078,11 @@
       </c>
       <c r="E25">
         <f t="shared" si="3"/>
-        <v>196</v>
+        <v>156</v>
       </c>
       <c r="K25" t="str">
         <f>_xlfn.CONCAT(E172, ", ", E173, ", ", E174, ", ", E175, ", ", E176, ", ", E177, ", ", E178, ", ", E179, ", ", E180, ", ", E181, ", ")</f>
-        <v xml:space="preserve">21, 20, 18, 17, 16, 14, 13, 12, 11, 10, </v>
+        <v xml:space="preserve">13, 12, 11, 10, 9, 8, 7, 6, 5, 4, </v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
@@ -3109,11 +3103,11 @@
       </c>
       <c r="E26">
         <f t="shared" si="3"/>
-        <v>199</v>
+        <v>158</v>
       </c>
       <c r="K26" t="str">
         <f>_xlfn.CONCAT(E182, ", ", E183, ", ", E184, ", ", E185, ", ", E186, ", ", E187, ", ", E188, ", ", E189, ", ", E190, ", ", E191, ", ")</f>
-        <v xml:space="preserve">9, 9, 8, 7, 7, 6, 6, 6, 5, 5, </v>
+        <v xml:space="preserve">4, 3, 2, 2, 1, 1, 1, 0, 0, 0, </v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
@@ -3134,11 +3128,11 @@
       </c>
       <c r="E27">
         <f t="shared" si="3"/>
-        <v>201</v>
+        <v>160</v>
       </c>
       <c r="K27" t="str">
         <f>_xlfn.CONCAT(E192, ", ", E193, ", ", E194, ", ", E195, ", ", E196, ", ", E197, ", ", E198, ", ", E199, ", ", E200, ", ", E201, ", ")</f>
-        <v xml:space="preserve">5, 5, 5, 5, 5, 6, 6, 6, 7, 7, </v>
+        <v xml:space="preserve">0, 0, 0, 0, 0, 0, 1, 1, 1, 2, </v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
@@ -3159,11 +3153,11 @@
       </c>
       <c r="E28">
         <f t="shared" si="3"/>
-        <v>204</v>
+        <v>162</v>
       </c>
       <c r="K28" t="str">
         <f>_xlfn.CONCAT(E202, ", ", E203, ", ", E204, ", ", E205, ", ", E206, ", ", E207, ", ", E208, ", ", E209, ", ", E210, ", ", E211, ", ")</f>
-        <v xml:space="preserve">8, 9, 9, 10, 11, 12, 13, 14, 16, 17, </v>
+        <v xml:space="preserve">2, 3, 4, 4, 5, 6, 7, 8, 9, 10, </v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
@@ -3184,11 +3178,11 @@
       </c>
       <c r="E29">
         <f t="shared" si="3"/>
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="K29" t="str">
         <f>_xlfn.CONCAT(E212, ", ", E213, ", ", E214, ", ", E215, ", ", E216, ", ", E217, ", ", E218, ", ", E219, ", ", E220, ", ", E221, ", ")</f>
-        <v xml:space="preserve">18, 20, 21, 22, 24, 26, 27, 29, 31, 33, </v>
+        <v xml:space="preserve">11, 12, 13, 14, 16, 17, 18, 20, 21, 23, </v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
@@ -3209,11 +3203,11 @@
       </c>
       <c r="E30">
         <f t="shared" si="3"/>
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="K30" t="str">
         <f>_xlfn.CONCAT(E222, ", ", E223, ", ", E224, ", ", E225, ", ", E226, ", ", E227, ", ", E228, ", ", E229, ", ", E230, ", ", E231, ", ")</f>
-        <v xml:space="preserve">35, 37, 39, 41, 43, 45, 48, 50, 52, 55, </v>
+        <v xml:space="preserve">24, 26, 28, 29, 31, 33, 35, 37, 38, 40, </v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
@@ -3234,11 +3228,11 @@
       </c>
       <c r="E31">
         <f t="shared" si="3"/>
-        <v>211</v>
+        <v>167</v>
       </c>
       <c r="K31" t="str">
         <f>_xlfn.CONCAT(E232, ", ", E233, ", ", E234, ", ", E235, ", ", E236, ", ", E237, ", ", E238, ", ", E239, ", ", E240, ", ", E241, ", ")</f>
-        <v xml:space="preserve">57, 60, 62, 65, 67, 70, 73, 75, 78, 81, </v>
+        <v xml:space="preserve">42, 44, 47, 49, 51, 53, 55, 57, 59, 62, </v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
@@ -3259,11 +3253,11 @@
       </c>
       <c r="E32">
         <f t="shared" si="3"/>
-        <v>213</v>
+        <v>169</v>
       </c>
       <c r="K32" t="str">
         <f>_xlfn.CONCAT(E242, ", ", E243, ", ", E244, ", ", E245, ", ", E246, ", ", E247, ", ", E248, ", ", E249, ", ", E250, ", ", E251, ", ")</f>
-        <v xml:space="preserve">84, 87, 89, 92, 95, 98, 101, 104, 107, 110, </v>
+        <v xml:space="preserve">64, 66, 69, 71, 73, 76, 78, 80, 83, 85, </v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
@@ -3284,11 +3278,11 @@
       </c>
       <c r="E33">
         <f t="shared" si="3"/>
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="K33" t="str">
         <f>_xlfn.CONCAT(E252, ", ", E253, ", ", E254, ", ", E255, ", ", E256, ", ", E257, "};")</f>
-        <v>113, 116, 119, 122, 125, 128};</v>
+        <v>88, 90, 93, 95, 98, 100};</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
@@ -3309,7 +3303,7 @@
       </c>
       <c r="E34">
         <f t="shared" si="3"/>
-        <v>217</v>
+        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
@@ -3330,7 +3324,7 @@
       </c>
       <c r="E35">
         <f t="shared" si="3"/>
-        <v>219</v>
+        <v>174</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
@@ -3351,7 +3345,7 @@
       </c>
       <c r="E36">
         <f t="shared" si="3"/>
-        <v>221</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
@@ -3372,7 +3366,7 @@
       </c>
       <c r="E37">
         <f t="shared" si="3"/>
-        <v>223</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
@@ -3393,7 +3387,7 @@
       </c>
       <c r="E38">
         <f t="shared" si="3"/>
-        <v>225</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
@@ -3414,7 +3408,7 @@
       </c>
       <c r="E39">
         <f t="shared" si="3"/>
-        <v>227</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
@@ -3435,7 +3429,7 @@
       </c>
       <c r="E40">
         <f t="shared" si="3"/>
-        <v>229</v>
+        <v>182</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
@@ -3456,7 +3450,7 @@
       </c>
       <c r="E41">
         <f t="shared" si="3"/>
-        <v>230</v>
+        <v>183</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
@@ -3477,7 +3471,7 @@
       </c>
       <c r="E42">
         <f t="shared" si="3"/>
-        <v>232</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
@@ -3498,7 +3492,7 @@
       </c>
       <c r="E43">
         <f t="shared" si="3"/>
-        <v>234</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
@@ -3519,7 +3513,7 @@
       </c>
       <c r="E44">
         <f t="shared" si="3"/>
-        <v>235</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
@@ -3540,7 +3534,7 @@
       </c>
       <c r="E45">
         <f t="shared" si="3"/>
-        <v>236</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
@@ -3561,7 +3555,7 @@
       </c>
       <c r="E46">
         <f t="shared" si="3"/>
-        <v>238</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
@@ -3582,7 +3576,7 @@
       </c>
       <c r="E47">
         <f t="shared" si="3"/>
-        <v>239</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
@@ -3603,7 +3597,7 @@
       </c>
       <c r="E48">
         <f t="shared" si="3"/>
-        <v>240</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -3624,7 +3618,7 @@
       </c>
       <c r="E49">
         <f t="shared" si="3"/>
-        <v>242</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -3645,7 +3639,7 @@
       </c>
       <c r="E50">
         <f t="shared" si="3"/>
-        <v>243</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -3666,7 +3660,7 @@
       </c>
       <c r="E51">
         <f t="shared" si="3"/>
-        <v>244</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -3687,7 +3681,7 @@
       </c>
       <c r="E52">
         <f t="shared" si="3"/>
-        <v>245</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -3708,7 +3702,7 @@
       </c>
       <c r="E53">
         <f t="shared" si="3"/>
-        <v>246</v>
+        <v>196</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -3729,7 +3723,7 @@
       </c>
       <c r="E54">
         <f t="shared" si="3"/>
-        <v>247</v>
+        <v>196</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -3750,7 +3744,7 @@
       </c>
       <c r="E55">
         <f t="shared" si="3"/>
-        <v>247</v>
+        <v>197</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -3771,7 +3765,7 @@
       </c>
       <c r="E56">
         <f t="shared" si="3"/>
-        <v>248</v>
+        <v>198</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -3792,7 +3786,7 @@
       </c>
       <c r="E57">
         <f t="shared" si="3"/>
-        <v>249</v>
+        <v>198</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -3813,7 +3807,7 @@
       </c>
       <c r="E58">
         <f t="shared" si="3"/>
-        <v>249</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -3834,7 +3828,7 @@
       </c>
       <c r="E59">
         <f t="shared" si="3"/>
-        <v>250</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -3855,7 +3849,7 @@
       </c>
       <c r="E60">
         <f t="shared" si="3"/>
-        <v>250</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -3876,7 +3870,7 @@
       </c>
       <c r="E61">
         <f t="shared" si="3"/>
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -3897,7 +3891,7 @@
       </c>
       <c r="E62">
         <f t="shared" si="3"/>
-        <v>251</v>
+        <v>200</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -3918,7 +3912,7 @@
       </c>
       <c r="E63">
         <f t="shared" si="3"/>
-        <v>251</v>
+        <v>200</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -3939,7 +3933,7 @@
       </c>
       <c r="E64">
         <f t="shared" si="3"/>
-        <v>251</v>
+        <v>200</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.3">
@@ -3960,7 +3954,7 @@
       </c>
       <c r="E65">
         <f t="shared" si="3"/>
-        <v>251</v>
+        <v>200</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.3">
@@ -3981,7 +3975,7 @@
       </c>
       <c r="E66">
         <f t="shared" si="3"/>
-        <v>251</v>
+        <v>200</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -4001,8 +3995,8 @@
         <v>0.99879545620517241</v>
       </c>
       <c r="E67">
-        <f t="shared" ref="E67:E130" si="7">ROUND(($J$4*(D67+1))+$J$3, 0)</f>
-        <v>251</v>
+        <f t="shared" ref="E67:E130" si="7">ROUND(($J$4*(D67))+$J$3, 0)</f>
+        <v>200</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.3">
@@ -4023,7 +4017,7 @@
       </c>
       <c r="E68">
         <f t="shared" si="7"/>
-        <v>251</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.3">
@@ -4044,7 +4038,7 @@
       </c>
       <c r="E69">
         <f t="shared" si="7"/>
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.3">
@@ -4065,7 +4059,7 @@
       </c>
       <c r="E70">
         <f t="shared" si="7"/>
-        <v>250</v>
+        <v>199</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -4086,7 +4080,7 @@
       </c>
       <c r="E71">
         <f t="shared" si="7"/>
-        <v>250</v>
+        <v>199</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
@@ -4107,7 +4101,7 @@
       </c>
       <c r="E72">
         <f t="shared" si="7"/>
-        <v>249</v>
+        <v>199</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -4128,7 +4122,7 @@
       </c>
       <c r="E73">
         <f t="shared" si="7"/>
-        <v>249</v>
+        <v>198</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -4149,7 +4143,7 @@
       </c>
       <c r="E74">
         <f t="shared" si="7"/>
-        <v>248</v>
+        <v>198</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -4170,7 +4164,7 @@
       </c>
       <c r="E75">
         <f t="shared" si="7"/>
-        <v>247</v>
+        <v>197</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -4191,7 +4185,7 @@
       </c>
       <c r="E76">
         <f t="shared" si="7"/>
-        <v>247</v>
+        <v>196</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.3">
@@ -4212,7 +4206,7 @@
       </c>
       <c r="E77">
         <f t="shared" si="7"/>
-        <v>246</v>
+        <v>196</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -4233,7 +4227,7 @@
       </c>
       <c r="E78">
         <f t="shared" si="7"/>
-        <v>245</v>
+        <v>195</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.3">
@@ -4254,7 +4248,7 @@
       </c>
       <c r="E79">
         <f t="shared" si="7"/>
-        <v>244</v>
+        <v>194</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.3">
@@ -4275,7 +4269,7 @@
       </c>
       <c r="E80">
         <f t="shared" si="7"/>
-        <v>243</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -4296,7 +4290,7 @@
       </c>
       <c r="E81">
         <f t="shared" si="7"/>
-        <v>242</v>
+        <v>192</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.3">
@@ -4317,7 +4311,7 @@
       </c>
       <c r="E82">
         <f t="shared" si="7"/>
-        <v>240</v>
+        <v>191</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.3">
@@ -4338,7 +4332,7 @@
       </c>
       <c r="E83">
         <f t="shared" si="7"/>
-        <v>239</v>
+        <v>190</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.3">
@@ -4359,7 +4353,7 @@
       </c>
       <c r="E84">
         <f t="shared" si="7"/>
-        <v>238</v>
+        <v>189</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.3">
@@ -4380,7 +4374,7 @@
       </c>
       <c r="E85">
         <f t="shared" si="7"/>
-        <v>236</v>
+        <v>188</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.3">
@@ -4401,7 +4395,7 @@
       </c>
       <c r="E86">
         <f t="shared" si="7"/>
-        <v>235</v>
+        <v>187</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -4422,7 +4416,7 @@
       </c>
       <c r="E87">
         <f t="shared" si="7"/>
-        <v>234</v>
+        <v>186</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.3">
@@ -4443,7 +4437,7 @@
       </c>
       <c r="E88">
         <f t="shared" si="7"/>
-        <v>232</v>
+        <v>184</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.3">
@@ -4464,7 +4458,7 @@
       </c>
       <c r="E89">
         <f t="shared" si="7"/>
-        <v>230</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.3">
@@ -4485,7 +4479,7 @@
       </c>
       <c r="E90">
         <f t="shared" si="7"/>
-        <v>229</v>
+        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
@@ -4506,7 +4500,7 @@
       </c>
       <c r="E91">
         <f t="shared" si="7"/>
-        <v>227</v>
+        <v>180</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
@@ -4527,7 +4521,7 @@
       </c>
       <c r="E92">
         <f t="shared" si="7"/>
-        <v>225</v>
+        <v>179</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.3">
@@ -4548,7 +4542,7 @@
       </c>
       <c r="E93">
         <f t="shared" si="7"/>
-        <v>223</v>
+        <v>177</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -4569,7 +4563,7 @@
       </c>
       <c r="E94">
         <f t="shared" si="7"/>
-        <v>221</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.3">
@@ -4590,7 +4584,7 @@
       </c>
       <c r="E95">
         <f t="shared" si="7"/>
-        <v>219</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.3">
@@ -4611,7 +4605,7 @@
       </c>
       <c r="E96">
         <f t="shared" si="7"/>
-        <v>217</v>
+        <v>172</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
@@ -4632,7 +4626,7 @@
       </c>
       <c r="E97">
         <f t="shared" si="7"/>
-        <v>215</v>
+        <v>171</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.3">
@@ -4653,7 +4647,7 @@
       </c>
       <c r="E98">
         <f t="shared" si="7"/>
-        <v>213</v>
+        <v>169</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
@@ -4674,7 +4668,7 @@
       </c>
       <c r="E99">
         <f t="shared" si="7"/>
-        <v>211</v>
+        <v>167</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -4695,7 +4689,7 @@
       </c>
       <c r="E100">
         <f t="shared" si="7"/>
-        <v>208</v>
+        <v>165</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
@@ -4716,7 +4710,7 @@
       </c>
       <c r="E101">
         <f t="shared" si="7"/>
-        <v>206</v>
+        <v>163</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
@@ -4737,7 +4731,7 @@
       </c>
       <c r="E102">
         <f t="shared" si="7"/>
-        <v>204</v>
+        <v>162</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.3">
@@ -4758,7 +4752,7 @@
       </c>
       <c r="E103">
         <f t="shared" si="7"/>
-        <v>201</v>
+        <v>160</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
@@ -4779,7 +4773,7 @@
       </c>
       <c r="E104">
         <f t="shared" si="7"/>
-        <v>199</v>
+        <v>158</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
@@ -4800,7 +4794,7 @@
       </c>
       <c r="E105">
         <f t="shared" si="7"/>
-        <v>196</v>
+        <v>156</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
@@ -4821,7 +4815,7 @@
       </c>
       <c r="E106">
         <f t="shared" si="7"/>
-        <v>194</v>
+        <v>153</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
@@ -4842,7 +4836,7 @@
       </c>
       <c r="E107">
         <f t="shared" si="7"/>
-        <v>191</v>
+        <v>151</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
@@ -4863,7 +4857,7 @@
       </c>
       <c r="E108">
         <f t="shared" si="7"/>
-        <v>189</v>
+        <v>149</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
@@ -4884,7 +4878,7 @@
       </c>
       <c r="E109">
         <f t="shared" si="7"/>
-        <v>186</v>
+        <v>147</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
@@ -4905,7 +4899,7 @@
       </c>
       <c r="E110">
         <f t="shared" si="7"/>
-        <v>183</v>
+        <v>145</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
@@ -4926,7 +4920,7 @@
       </c>
       <c r="E111">
         <f t="shared" si="7"/>
-        <v>181</v>
+        <v>143</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
@@ -4947,7 +4941,7 @@
       </c>
       <c r="E112">
         <f t="shared" si="7"/>
-        <v>178</v>
+        <v>141</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
@@ -4968,7 +4962,7 @@
       </c>
       <c r="E113">
         <f t="shared" si="7"/>
-        <v>175</v>
+        <v>138</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
@@ -4989,7 +4983,7 @@
       </c>
       <c r="E114">
         <f t="shared" si="7"/>
-        <v>172</v>
+        <v>136</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
@@ -5010,7 +5004,7 @@
       </c>
       <c r="E115">
         <f t="shared" si="7"/>
-        <v>169</v>
+        <v>134</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
@@ -5031,7 +5025,7 @@
       </c>
       <c r="E116">
         <f t="shared" si="7"/>
-        <v>167</v>
+        <v>131</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
@@ -5052,7 +5046,7 @@
       </c>
       <c r="E117">
         <f t="shared" si="7"/>
-        <v>164</v>
+        <v>129</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
@@ -5073,7 +5067,7 @@
       </c>
       <c r="E118">
         <f t="shared" si="7"/>
-        <v>161</v>
+        <v>127</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
@@ -5094,7 +5088,7 @@
       </c>
       <c r="E119">
         <f t="shared" si="7"/>
-        <v>158</v>
+        <v>124</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
@@ -5115,7 +5109,7 @@
       </c>
       <c r="E120">
         <f t="shared" si="7"/>
-        <v>155</v>
+        <v>122</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
@@ -5136,7 +5130,7 @@
       </c>
       <c r="E121">
         <f t="shared" si="7"/>
-        <v>152</v>
+        <v>120</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
@@ -5157,7 +5151,7 @@
       </c>
       <c r="E122">
         <f t="shared" si="7"/>
-        <v>149</v>
+        <v>117</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
@@ -5178,7 +5172,7 @@
       </c>
       <c r="E123">
         <f t="shared" si="7"/>
-        <v>146</v>
+        <v>115</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
@@ -5199,7 +5193,7 @@
       </c>
       <c r="E124">
         <f t="shared" si="7"/>
-        <v>143</v>
+        <v>112</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
@@ -5220,7 +5214,7 @@
       </c>
       <c r="E125">
         <f t="shared" si="7"/>
-        <v>140</v>
+        <v>110</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
@@ -5241,7 +5235,7 @@
       </c>
       <c r="E126">
         <f t="shared" si="7"/>
-        <v>137</v>
+        <v>107</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -5262,7 +5256,7 @@
       </c>
       <c r="E127">
         <f t="shared" si="7"/>
-        <v>134</v>
+        <v>105</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
@@ -5283,7 +5277,7 @@
       </c>
       <c r="E128">
         <f t="shared" si="7"/>
-        <v>131</v>
+        <v>102</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
@@ -5304,7 +5298,7 @@
       </c>
       <c r="E129">
         <f t="shared" si="7"/>
-        <v>128</v>
+        <v>100</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
@@ -5325,7 +5319,7 @@
       </c>
       <c r="E130">
         <f t="shared" si="7"/>
-        <v>125</v>
+        <v>98</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
@@ -5345,8 +5339,8 @@
         <v>-4.9067674327418168E-2</v>
       </c>
       <c r="E131">
-        <f t="shared" ref="E131:E194" si="11">ROUND(($J$4*(D131+1))+$J$3, 0)</f>
-        <v>122</v>
+        <f t="shared" ref="E131:E194" si="11">ROUND(($J$4*(D131))+$J$3, 0)</f>
+        <v>95</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
@@ -5367,7 +5361,7 @@
       </c>
       <c r="E132">
         <f t="shared" si="11"/>
-        <v>119</v>
+        <v>93</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
@@ -5388,7 +5382,7 @@
       </c>
       <c r="E133">
         <f t="shared" si="11"/>
-        <v>116</v>
+        <v>90</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
@@ -5409,7 +5403,7 @@
       </c>
       <c r="E134">
         <f t="shared" si="11"/>
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
@@ -5430,7 +5424,7 @@
       </c>
       <c r="E135">
         <f t="shared" si="11"/>
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
@@ -5451,7 +5445,7 @@
       </c>
       <c r="E136">
         <f t="shared" si="11"/>
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
@@ -5472,7 +5466,7 @@
       </c>
       <c r="E137">
         <f t="shared" si="11"/>
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
@@ -5493,7 +5487,7 @@
       </c>
       <c r="E138">
         <f t="shared" si="11"/>
-        <v>101</v>
+        <v>78</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
@@ -5514,7 +5508,7 @@
       </c>
       <c r="E139">
         <f t="shared" si="11"/>
-        <v>98</v>
+        <v>76</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
@@ -5535,7 +5529,7 @@
       </c>
       <c r="E140">
         <f t="shared" si="11"/>
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
@@ -5556,7 +5550,7 @@
       </c>
       <c r="E141">
         <f t="shared" si="11"/>
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
@@ -5577,7 +5571,7 @@
       </c>
       <c r="E142">
         <f t="shared" si="11"/>
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
@@ -5598,7 +5592,7 @@
       </c>
       <c r="E143">
         <f t="shared" si="11"/>
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
@@ -5619,7 +5613,7 @@
       </c>
       <c r="E144">
         <f t="shared" si="11"/>
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
@@ -5640,7 +5634,7 @@
       </c>
       <c r="E145">
         <f t="shared" si="11"/>
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
@@ -5661,7 +5655,7 @@
       </c>
       <c r="E146">
         <f t="shared" si="11"/>
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
@@ -5682,7 +5676,7 @@
       </c>
       <c r="E147">
         <f t="shared" si="11"/>
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
@@ -5703,7 +5697,7 @@
       </c>
       <c r="E148">
         <f t="shared" si="11"/>
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
@@ -5724,7 +5718,7 @@
       </c>
       <c r="E149">
         <f t="shared" si="11"/>
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
@@ -5745,7 +5739,7 @@
       </c>
       <c r="E150">
         <f t="shared" si="11"/>
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
@@ -5766,7 +5760,7 @@
       </c>
       <c r="E151">
         <f t="shared" si="11"/>
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
@@ -5787,7 +5781,7 @@
       </c>
       <c r="E152">
         <f t="shared" si="11"/>
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
@@ -5808,7 +5802,7 @@
       </c>
       <c r="E153">
         <f t="shared" si="11"/>
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
@@ -5829,7 +5823,7 @@
       </c>
       <c r="E154">
         <f t="shared" si="11"/>
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
@@ -5850,7 +5844,7 @@
       </c>
       <c r="E155">
         <f t="shared" si="11"/>
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
@@ -5871,7 +5865,7 @@
       </c>
       <c r="E156">
         <f t="shared" si="11"/>
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
@@ -5892,7 +5886,7 @@
       </c>
       <c r="E157">
         <f t="shared" si="11"/>
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
@@ -5913,7 +5907,7 @@
       </c>
       <c r="E158">
         <f t="shared" si="11"/>
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
@@ -5934,7 +5928,7 @@
       </c>
       <c r="E159">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
@@ -5955,7 +5949,7 @@
       </c>
       <c r="E160">
         <f t="shared" si="11"/>
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
@@ -5976,7 +5970,7 @@
       </c>
       <c r="E161">
         <f t="shared" si="11"/>
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.3">
@@ -5997,7 +5991,7 @@
       </c>
       <c r="E162">
         <f t="shared" si="11"/>
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
@@ -6018,7 +6012,7 @@
       </c>
       <c r="E163">
         <f t="shared" si="11"/>
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
@@ -6039,7 +6033,7 @@
       </c>
       <c r="E164">
         <f t="shared" si="11"/>
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
@@ -6060,7 +6054,7 @@
       </c>
       <c r="E165">
         <f t="shared" si="11"/>
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
@@ -6081,7 +6075,7 @@
       </c>
       <c r="E166">
         <f t="shared" si="11"/>
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
@@ -6102,7 +6096,7 @@
       </c>
       <c r="E167">
         <f t="shared" si="11"/>
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
@@ -6123,7 +6117,7 @@
       </c>
       <c r="E168">
         <f t="shared" si="11"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
@@ -6144,7 +6138,7 @@
       </c>
       <c r="E169">
         <f t="shared" si="11"/>
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
@@ -6165,7 +6159,7 @@
       </c>
       <c r="E170">
         <f t="shared" si="11"/>
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
@@ -6186,7 +6180,7 @@
       </c>
       <c r="E171">
         <f t="shared" si="11"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
@@ -6207,7 +6201,7 @@
       </c>
       <c r="E172">
         <f t="shared" si="11"/>
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
@@ -6228,7 +6222,7 @@
       </c>
       <c r="E173">
         <f t="shared" si="11"/>
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
@@ -6249,7 +6243,7 @@
       </c>
       <c r="E174">
         <f t="shared" si="11"/>
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
@@ -6270,7 +6264,7 @@
       </c>
       <c r="E175">
         <f t="shared" si="11"/>
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
@@ -6291,7 +6285,7 @@
       </c>
       <c r="E176">
         <f t="shared" si="11"/>
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
@@ -6312,7 +6306,7 @@
       </c>
       <c r="E177">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
@@ -6333,7 +6327,7 @@
       </c>
       <c r="E178">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
@@ -6354,7 +6348,7 @@
       </c>
       <c r="E179">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
@@ -6375,7 +6369,7 @@
       </c>
       <c r="E180">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
@@ -6396,7 +6390,7 @@
       </c>
       <c r="E181">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
@@ -6417,7 +6411,7 @@
       </c>
       <c r="E182">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
@@ -6438,7 +6432,7 @@
       </c>
       <c r="E183">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
@@ -6459,7 +6453,7 @@
       </c>
       <c r="E184">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
@@ -6480,7 +6474,7 @@
       </c>
       <c r="E185">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
@@ -6501,7 +6495,7 @@
       </c>
       <c r="E186">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
@@ -6522,7 +6516,7 @@
       </c>
       <c r="E187">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
@@ -6543,7 +6537,7 @@
       </c>
       <c r="E188">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
@@ -6564,7 +6558,7 @@
       </c>
       <c r="E189">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
@@ -6585,7 +6579,7 @@
       </c>
       <c r="E190">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
@@ -6606,7 +6600,7 @@
       </c>
       <c r="E191">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
@@ -6627,7 +6621,7 @@
       </c>
       <c r="E192">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
@@ -6648,7 +6642,7 @@
       </c>
       <c r="E193">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
@@ -6669,7 +6663,7 @@
       </c>
       <c r="E194">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
@@ -6689,8 +6683,8 @@
         <v>-0.99879545620517241</v>
       </c>
       <c r="E195">
-        <f t="shared" ref="E195:E257" si="15">ROUND(($J$4*(D195+1))+$J$3, 0)</f>
-        <v>5</v>
+        <f t="shared" ref="E195:E257" si="15">ROUND(($J$4*(D195))+$J$3, 0)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
@@ -6711,7 +6705,7 @@
       </c>
       <c r="E196">
         <f t="shared" si="15"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
@@ -6732,7 +6726,7 @@
       </c>
       <c r="E197">
         <f t="shared" si="15"/>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
@@ -6753,7 +6747,7 @@
       </c>
       <c r="E198">
         <f t="shared" si="15"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
@@ -6774,7 +6768,7 @@
       </c>
       <c r="E199">
         <f t="shared" si="15"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
@@ -6795,7 +6789,7 @@
       </c>
       <c r="E200">
         <f t="shared" si="15"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
@@ -6816,7 +6810,7 @@
       </c>
       <c r="E201">
         <f t="shared" si="15"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
@@ -6837,7 +6831,7 @@
       </c>
       <c r="E202">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
@@ -6858,7 +6852,7 @@
       </c>
       <c r="E203">
         <f t="shared" si="15"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.3">
@@ -6879,7 +6873,7 @@
       </c>
       <c r="E204">
         <f t="shared" si="15"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
@@ -6900,7 +6894,7 @@
       </c>
       <c r="E205">
         <f t="shared" si="15"/>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
@@ -6921,7 +6915,7 @@
       </c>
       <c r="E206">
         <f t="shared" si="15"/>
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
@@ -6942,7 +6936,7 @@
       </c>
       <c r="E207">
         <f t="shared" si="15"/>
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
@@ -6963,7 +6957,7 @@
       </c>
       <c r="E208">
         <f t="shared" si="15"/>
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
@@ -6984,7 +6978,7 @@
       </c>
       <c r="E209">
         <f t="shared" si="15"/>
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
@@ -7005,7 +6999,7 @@
       </c>
       <c r="E210">
         <f t="shared" si="15"/>
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
@@ -7026,7 +7020,7 @@
       </c>
       <c r="E211">
         <f t="shared" si="15"/>
-        <v>17</v>
+        <v>10</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
@@ -7047,7 +7041,7 @@
       </c>
       <c r="E212">
         <f t="shared" si="15"/>
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
@@ -7068,7 +7062,7 @@
       </c>
       <c r="E213">
         <f t="shared" si="15"/>
-        <v>20</v>
+        <v>12</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
@@ -7089,7 +7083,7 @@
       </c>
       <c r="E214">
         <f t="shared" si="15"/>
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
@@ -7110,7 +7104,7 @@
       </c>
       <c r="E215">
         <f t="shared" si="15"/>
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
@@ -7131,7 +7125,7 @@
       </c>
       <c r="E216">
         <f t="shared" si="15"/>
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
@@ -7152,7 +7146,7 @@
       </c>
       <c r="E217">
         <f t="shared" si="15"/>
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
@@ -7173,7 +7167,7 @@
       </c>
       <c r="E218">
         <f t="shared" si="15"/>
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
@@ -7194,7 +7188,7 @@
       </c>
       <c r="E219">
         <f t="shared" si="15"/>
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
@@ -7215,7 +7209,7 @@
       </c>
       <c r="E220">
         <f t="shared" si="15"/>
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
@@ -7236,7 +7230,7 @@
       </c>
       <c r="E221">
         <f t="shared" si="15"/>
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
@@ -7257,7 +7251,7 @@
       </c>
       <c r="E222">
         <f t="shared" si="15"/>
-        <v>35</v>
+        <v>24</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
@@ -7278,7 +7272,7 @@
       </c>
       <c r="E223">
         <f t="shared" si="15"/>
-        <v>37</v>
+        <v>26</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
@@ -7299,7 +7293,7 @@
       </c>
       <c r="E224">
         <f t="shared" si="15"/>
-        <v>39</v>
+        <v>28</v>
       </c>
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
@@ -7320,7 +7314,7 @@
       </c>
       <c r="E225">
         <f t="shared" si="15"/>
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
@@ -7341,7 +7335,7 @@
       </c>
       <c r="E226">
         <f t="shared" si="15"/>
-        <v>43</v>
+        <v>31</v>
       </c>
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
@@ -7362,7 +7356,7 @@
       </c>
       <c r="E227">
         <f t="shared" si="15"/>
-        <v>45</v>
+        <v>33</v>
       </c>
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
@@ -7383,7 +7377,7 @@
       </c>
       <c r="E228">
         <f t="shared" si="15"/>
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
@@ -7404,7 +7398,7 @@
       </c>
       <c r="E229">
         <f t="shared" si="15"/>
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
@@ -7425,7 +7419,7 @@
       </c>
       <c r="E230">
         <f t="shared" si="15"/>
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
@@ -7446,7 +7440,7 @@
       </c>
       <c r="E231">
         <f t="shared" si="15"/>
-        <v>55</v>
+        <v>40</v>
       </c>
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
@@ -7467,7 +7461,7 @@
       </c>
       <c r="E232">
         <f t="shared" si="15"/>
-        <v>57</v>
+        <v>42</v>
       </c>
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
@@ -7488,7 +7482,7 @@
       </c>
       <c r="E233">
         <f t="shared" si="15"/>
-        <v>60</v>
+        <v>44</v>
       </c>
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
@@ -7509,7 +7503,7 @@
       </c>
       <c r="E234">
         <f t="shared" si="15"/>
-        <v>62</v>
+        <v>47</v>
       </c>
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.3">
@@ -7530,7 +7524,7 @@
       </c>
       <c r="E235">
         <f t="shared" si="15"/>
-        <v>65</v>
+        <v>49</v>
       </c>
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.3">
@@ -7551,7 +7545,7 @@
       </c>
       <c r="E236">
         <f t="shared" si="15"/>
-        <v>67</v>
+        <v>51</v>
       </c>
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.3">
@@ -7572,7 +7566,7 @@
       </c>
       <c r="E237">
         <f t="shared" si="15"/>
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
@@ -7593,7 +7587,7 @@
       </c>
       <c r="E238">
         <f t="shared" si="15"/>
-        <v>73</v>
+        <v>55</v>
       </c>
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
@@ -7614,7 +7608,7 @@
       </c>
       <c r="E239">
         <f t="shared" si="15"/>
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
@@ -7635,7 +7629,7 @@
       </c>
       <c r="E240">
         <f t="shared" si="15"/>
-        <v>78</v>
+        <v>59</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
@@ -7656,7 +7650,7 @@
       </c>
       <c r="E241">
         <f t="shared" si="15"/>
-        <v>81</v>
+        <v>62</v>
       </c>
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.3">
@@ -7677,7 +7671,7 @@
       </c>
       <c r="E242">
         <f t="shared" si="15"/>
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.3">
@@ -7698,7 +7692,7 @@
       </c>
       <c r="E243">
         <f t="shared" si="15"/>
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
@@ -7719,7 +7713,7 @@
       </c>
       <c r="E244">
         <f t="shared" si="15"/>
-        <v>89</v>
+        <v>69</v>
       </c>
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
@@ -7740,7 +7734,7 @@
       </c>
       <c r="E245">
         <f t="shared" si="15"/>
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
@@ -7761,7 +7755,7 @@
       </c>
       <c r="E246">
         <f t="shared" si="15"/>
-        <v>95</v>
+        <v>73</v>
       </c>
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
@@ -7782,7 +7776,7 @@
       </c>
       <c r="E247">
         <f t="shared" si="15"/>
-        <v>98</v>
+        <v>76</v>
       </c>
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
@@ -7803,7 +7797,7 @@
       </c>
       <c r="E248">
         <f t="shared" si="15"/>
-        <v>101</v>
+        <v>78</v>
       </c>
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
@@ -7824,7 +7818,7 @@
       </c>
       <c r="E249">
         <f t="shared" si="15"/>
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
@@ -7845,7 +7839,7 @@
       </c>
       <c r="E250">
         <f t="shared" si="15"/>
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
@@ -7866,7 +7860,7 @@
       </c>
       <c r="E251">
         <f t="shared" si="15"/>
-        <v>110</v>
+        <v>85</v>
       </c>
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
@@ -7887,7 +7881,7 @@
       </c>
       <c r="E252">
         <f t="shared" si="15"/>
-        <v>113</v>
+        <v>88</v>
       </c>
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.3">
@@ -7908,7 +7902,7 @@
       </c>
       <c r="E253">
         <f t="shared" si="15"/>
-        <v>116</v>
+        <v>90</v>
       </c>
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
@@ -7929,7 +7923,7 @@
       </c>
       <c r="E254">
         <f t="shared" si="15"/>
-        <v>119</v>
+        <v>93</v>
       </c>
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
@@ -7950,7 +7944,7 @@
       </c>
       <c r="E255">
         <f t="shared" si="15"/>
-        <v>122</v>
+        <v>95</v>
       </c>
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
@@ -7971,7 +7965,7 @@
       </c>
       <c r="E256">
         <f t="shared" si="15"/>
-        <v>125</v>
+        <v>98</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.3">
@@ -7992,7 +7986,7 @@
       </c>
       <c r="E257">
         <f t="shared" si="15"/>
-        <v>128</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added courtesy tone support. Firmware v0.9.9 which is a potential release candidate for 1.0.0.
</commit_message>
<xml_diff>
--- a/Timer Value Comparisons for Baud and Tone Generation.xlsx
+++ b/Timer Value Comparisons for Baud and Tone Generation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15da9958d5653d7c/Git/ptSolar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="142" documentId="8_{EFBF5CDD-90CD-49C6-81E3-4432BDE0BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F269326F-6C16-42C2-A719-242A8B3BF296}"/>
+  <xr:revisionPtr revIDLastSave="162" documentId="8_{EFBF5CDD-90CD-49C6-81E3-4432BDE0BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B4A1F94-46A1-4877-975A-08C5BB4359E9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="2" xr2:uid="{DF6E09ED-C946-4170-A532-3478E12C41B6}"/>
+    <workbookView xWindow="-30840" yWindow="-120" windowWidth="30960" windowHeight="16800" activeTab="2" xr2:uid="{DF6E09ED-C946-4170-A532-3478E12C41B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Truncated to 128" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>BG</t>
   </si>
@@ -94,6 +94,18 @@
   <si>
     <t>(set to 255 or less). This need to be at or less than the value in OCR2A or else you'll have overflow issues in the PWM generation.</t>
   </si>
+  <si>
+    <t>TONE_COURTESY</t>
+  </si>
+  <si>
+    <t>Low Tone</t>
+  </si>
+  <si>
+    <t>High Tone</t>
+  </si>
+  <si>
+    <t>Courtesy Tone</t>
+  </si>
 </sst>
 </file>
 
@@ -111,12 +123,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,9 +149,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4712,10 +4731,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED4B8AD3-CD47-4B54-BDA7-EF9D63D27F55}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4725,9 +4744,10 @@
     <col min="5" max="5" width="8.85546875" style="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4749,8 +4769,11 @@
       <c r="G1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20</v>
       </c>
@@ -4771,15 +4794,19 @@
         <v>1.0010010010010895E-3</v>
       </c>
       <c r="F2">
-        <f>ROUND(((65536*C2*2200) / 8000000), 0)</f>
+        <f>ROUND(((65536*C2*$N$4) / 8000000), 0)</f>
         <v>6001</v>
       </c>
       <c r="G2">
-        <f>ROUND(((65536*C2*1200) / 8000000), 0)</f>
+        <f>ROUND(((65536*C2*$N$3) / 8000000), 0)</f>
         <v>3274</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f>ROUND(((65536*C2*$N$5) / 8000000), 0)</f>
+        <v>4637</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>21</v>
       </c>
@@ -4800,27 +4827,37 @@
         <v>1.4521055530520854E-3</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F18" si="4">ROUND(((65536*C3*2200) / 8000000), 0)</f>
+        <f t="shared" ref="F3:F18" si="4">ROUND(((65536*C3*$N$4) / 8000000), 0)</f>
         <v>5713</v>
       </c>
       <c r="G3">
-        <f t="shared" ref="G3:G18" si="5">ROUND(((65536*C3*1200) / 8000000), 0)</f>
+        <f t="shared" ref="G3:G18" si="5">ROUND(((65536*C3*$N$3) / 8000000), 0)</f>
         <v>3116</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="H3">
+        <f t="shared" ref="H3:H18" si="6">ROUND(((65536*C3*$N$5) / 8000000), 0)</f>
+        <v>4415</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
         <v>22</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <f t="shared" si="0"/>
         <v>303.030303030303</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <f t="shared" si="1"/>
         <v>303</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <f t="shared" si="2"/>
         <v>1200.1200120012002</v>
       </c>
@@ -4828,16 +4865,26 @@
         <f t="shared" si="3"/>
         <v>1.0001000100023916E-4</v>
       </c>
-      <c r="F4">
-        <f>ROUND(((65536*C4*2200) / 8000000), 0)</f>
+      <c r="F4" s="2">
+        <f t="shared" si="4"/>
         <v>5461</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <f t="shared" si="5"/>
         <v>2979</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="2">
+        <f t="shared" si="6"/>
+        <v>4220</v>
+      </c>
+      <c r="M4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>23</v>
       </c>
@@ -4865,8 +4912,18 @@
         <f t="shared" si="5"/>
         <v>2851</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="6"/>
+        <v>4039</v>
+      </c>
+      <c r="M5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>24</v>
       </c>
@@ -4894,8 +4951,12 @@
         <f t="shared" si="5"/>
         <v>2733</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="6"/>
+        <v>3872</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>25</v>
       </c>
@@ -4923,8 +4984,12 @@
         <f t="shared" si="5"/>
         <v>2625</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="6"/>
+        <v>3718</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>26</v>
       </c>
@@ -4952,8 +5017,12 @@
         <f t="shared" si="5"/>
         <v>2517</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="6"/>
+        <v>3565</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>27</v>
       </c>
@@ -4981,8 +5050,12 @@
         <f t="shared" si="5"/>
         <v>2428</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" si="6"/>
+        <v>3440</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>28</v>
       </c>
@@ -5010,8 +5083,12 @@
         <f t="shared" si="5"/>
         <v>2340</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="6"/>
+        <v>3314</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>29</v>
       </c>
@@ -5039,8 +5116,12 @@
         <f t="shared" si="5"/>
         <v>2261</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="6"/>
+        <v>3203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>30</v>
       </c>
@@ -5068,8 +5149,12 @@
         <f t="shared" si="5"/>
         <v>2182</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f t="shared" si="6"/>
+        <v>3092</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>31</v>
       </c>
@@ -5097,8 +5182,12 @@
         <f t="shared" si="5"/>
         <v>2114</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f t="shared" si="6"/>
+        <v>2994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>32</v>
       </c>
@@ -5126,8 +5215,12 @@
         <f t="shared" si="5"/>
         <v>2045</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <f t="shared" si="6"/>
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>33</v>
       </c>
@@ -5155,8 +5248,12 @@
         <f t="shared" si="5"/>
         <v>1986</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <f t="shared" si="6"/>
+        <v>2813</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>34</v>
       </c>
@@ -5184,8 +5281,12 @@
         <f t="shared" si="5"/>
         <v>1927</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f t="shared" si="6"/>
+        <v>2730</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>35</v>
       </c>
@@ -5213,8 +5314,12 @@
         <f t="shared" si="5"/>
         <v>1868</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <f t="shared" si="6"/>
+        <v>2646</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>36</v>
       </c>
@@ -5241,6 +5346,10 @@
       <c r="G18">
         <f t="shared" si="5"/>
         <v>1819</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="6"/>
+        <v>2576</v>
       </c>
     </row>
   </sheetData>

</xml_diff>